<commit_message>
some model changes, some new url(update, delete, create)
</commit_message>
<xml_diff>
--- a/algorithm/result.xlsx
+++ b/algorithm/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>cost_of_time</t>
   </si>
@@ -40,37 +40,172 @@
     <t>v1</t>
   </si>
   <si>
-    <t>N38-81-N38</t>
-  </si>
-  <si>
-    <t>(627, 627)-(630, 634)-(637, 637)</t>
+    <t>N38-809-801-777-737-401-185-169-113-17-N38</t>
+  </si>
+  <si>
+    <t>(534, 534)-(535, 539)-(539, 543)-(550, 554)-(575, 579)-(665, 669)-(750, 754)-(755, 759)-(780, 784)-(820, 824)-(826, 826)</t>
   </si>
   <si>
     <t>v2</t>
   </si>
   <si>
-    <t>N38-193-177-169-161-121-129-89-49-1-N38</t>
-  </si>
-  <si>
-    <t>(524, 524)-(525, 529)-(535, 539)-(539, 543)-(580, 584)-(620, 624)-(625, 629)-(631, 635)-(700, 704)-(785, 789)-(791, 791)</t>
+    <t>N38-633-625-585-425-385-353-313-145-N38</t>
+  </si>
+  <si>
+    <t>(614, 614)-(615, 619)-(619, 623)-(625, 629)-(650, 654)-(665, 669)-(690, 694)-(710, 714)-(765, 769)-(771, 771)</t>
   </si>
   <si>
     <t>v3</t>
   </si>
   <si>
-    <t>N38-201-153-145-137-105-113-N38</t>
-  </si>
-  <si>
-    <t>(518, 518)-(520, 524)-(580, 584)-(585, 589)-(590, 594)-(625, 629)-(631, 635)-(636, 636)</t>
+    <t>N38-753-97-N38</t>
+  </si>
+  <si>
+    <t>(568, 568)-(570, 574)-(790, 794)-(796, 796)</t>
   </si>
   <si>
     <t>v4</t>
   </si>
   <si>
-    <t>N38-185-97-73-65-57-41-33-25-17-9-N38</t>
-  </si>
-  <si>
-    <t>(524, 524)-(525, 529)-(630, 634)-(635, 639)-(639, 643)-(685, 689)-(710, 714)-(715, 719)-(720, 724)-(745, 749)-(750, 754)-(756, 756)</t>
+    <t>N38-833-785-729-705-697-617-369-129-137-41-N38</t>
+  </si>
+  <si>
+    <t>(518, 518)-(520, 524)-(545, 549)-(580, 584)-(585, 589)-(590, 594)-(620, 624)-(685, 689)-(770, 774)-(775, 779)-(810, 814)-(816, 816)</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>N38-857-537-489-329-N38</t>
+  </si>
+  <si>
+    <t>(498, 498)-(500, 504)-(630, 634)-(645, 649)-(705, 709)-(711, 711)</t>
+  </si>
+  <si>
+    <t>v6</t>
+  </si>
+  <si>
+    <t>N38-713-681-689-609-345-297-305-265-81-N38</t>
+  </si>
+  <si>
+    <t>(578, 578)-(580, 584)-(595, 599)-(600, 604)-(620, 624)-(690, 694)-(710, 714)-(715, 719)-(720, 724)-(790, 794)-(796, 796)</t>
+  </si>
+  <si>
+    <t>v7</t>
+  </si>
+  <si>
+    <t>N38-841-521-529-393-233-225-N38</t>
+  </si>
+  <si>
+    <t>(518, 518)-(520, 524)-(635, 639)-(639, 643)-(665, 669)-(735, 739)-(740, 744)-(746, 746)</t>
+  </si>
+  <si>
+    <t>v8</t>
+  </si>
+  <si>
+    <t>N38-793-721-641-449-321-249-153-N38</t>
+  </si>
+  <si>
+    <t>(543, 543)-(545, 549)-(580, 584)-(610, 614)-(650, 654)-(705, 709)-(730, 734)-(765, 769)-(772, 772)</t>
+  </si>
+  <si>
+    <t>v9</t>
+  </si>
+  <si>
+    <t>N38-121-65-49-N38</t>
+  </si>
+  <si>
+    <t>(778, 778)-(780, 784)-(800, 804)-(805, 809)-(811, 811)</t>
+  </si>
+  <si>
+    <t>v10</t>
+  </si>
+  <si>
+    <t>N38-817-457-465-N38</t>
+  </si>
+  <si>
+    <t>(524, 524)-(525, 529)-(650, 654)-(655, 659)-(661, 661)</t>
+  </si>
+  <si>
+    <t>v11</t>
+  </si>
+  <si>
+    <t>N38-745-665-657-577-193-N38</t>
+  </si>
+  <si>
+    <t>(573, 573)-(575, 579)-(600, 604)-(605, 609)-(630, 634)-(750, 754)-(756, 756)</t>
+  </si>
+  <si>
+    <t>v12</t>
+  </si>
+  <si>
+    <t>N38-417-441-257-241-33-9-1-N38</t>
+  </si>
+  <si>
+    <t>(648, 648)-(650, 654)-(655, 659)-(725, 729)-(735, 739)-(815, 819)-(830, 834)-(835, 839)-(841, 841)</t>
+  </si>
+  <si>
+    <t>v13</t>
+  </si>
+  <si>
+    <t>N38-513-57-N38</t>
+  </si>
+  <si>
+    <t>(638, 638)-(640, 644)-(800, 804)-(806, 806)</t>
+  </si>
+  <si>
+    <t>v14</t>
+  </si>
+  <si>
+    <t>N38-825-561-273-209-N38</t>
+  </si>
+  <si>
+    <t>(524, 524)-(525, 529)-(630, 634)-(720, 724)-(740, 744)-(745, 745)</t>
+  </si>
+  <si>
+    <t>v15</t>
+  </si>
+  <si>
+    <t>N38-481-473-409-337-161-105-89-73-25-N38</t>
+  </si>
+  <si>
+    <t>(642, 642)-(645, 649)-(650, 654)-(655, 659)-(700, 704)-(760, 764)-(785, 789)-(790, 794)-(794, 798)-(815, 819)-(821, 821)</t>
+  </si>
+  <si>
+    <t>v16</t>
+  </si>
+  <si>
+    <t>N38-849-673-649-601-545-569-289-281-N38</t>
+  </si>
+  <si>
+    <t>(519, 519)-(520, 524)-(595, 599)-(610, 614)-(625, 629)-(630, 634)-(636, 640)-(710, 714)-(715, 719)-(720, 720)</t>
+  </si>
+  <si>
+    <t>v17</t>
+  </si>
+  <si>
+    <t>N38-769-761-377-217-N38</t>
+  </si>
+  <si>
+    <t>(548, 548)-(550, 554)-(565, 569)-(685, 689)-(740, 744)-(745, 745)</t>
+  </si>
+  <si>
+    <t>v18</t>
+  </si>
+  <si>
+    <t>N38-593-505-361-N38</t>
+  </si>
+  <si>
+    <t>(624, 624)-(625, 629)-(640, 644)-(690, 694)-(696, 696)</t>
+  </si>
+  <si>
+    <t>v19</t>
+  </si>
+  <si>
+    <t>N38-553-497-433-201-177-N38</t>
+  </si>
+  <si>
+    <t>(628, 628)-(630, 634)-(640, 644)-(650, 654)-(745, 749)-(750, 754)-(756, 756)</t>
   </si>
 </sst>
 </file>
@@ -402,7 +537,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -424,16 +559,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>147</v>
+        <v>590</v>
       </c>
       <c r="B2">
-        <v>11778.7442</v>
+        <v>46811.12729999999</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>147</v>
+        <v>590</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -489,6 +624,171 @@
       </c>
       <c r="C7" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>